<commit_message>
[feat] - find best combinations
</commit_message>
<xml_diff>
--- a/src/main/resources/Boards Cutter template.xlsx
+++ b/src/main/resources/Boards Cutter template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Igor\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Igor\Programming\Boards Cutter\BoardsCutter\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A37014-D9F7-453C-A707-67A475377E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E78497-147A-49A6-B873-07764E8254DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -563,9 +563,6 @@
     <xf numFmtId="1" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -585,6 +582,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -876,8 +876,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D2" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -896,30 +896,30 @@
   <sheetData>
     <row r="1" spans="2:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-      <c r="G2" s="28"/>
-      <c r="H2" s="28"/>
-      <c r="I2" s="28"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
     </row>
     <row r="3" spans="2:18" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="28" t="s">
+      <c r="B3" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28" t="s">
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
     </row>
     <row r="4" spans="2:18" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
@@ -946,7 +946,7 @@
       <c r="I4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="32" t="s">
+      <c r="K4" s="31" t="s">
         <v>22</v>
       </c>
       <c r="L4" s="5" t="s">
@@ -979,10 +979,10 @@
       <c r="I5" s="23">
         <v>15</v>
       </c>
-      <c r="K5" s="31" t="s">
+      <c r="K5" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="L5" s="33">
+      <c r="L5" s="32">
         <v>0</v>
       </c>
       <c r="R5" s="3" t="s">
@@ -1016,8 +1016,8 @@
       <c r="I6" s="25">
         <v>15</v>
       </c>
-      <c r="K6" s="29"/>
-      <c r="L6" s="34"/>
+      <c r="K6" s="28"/>
+      <c r="L6" s="33"/>
       <c r="R6" s="3" t="s">
         <v>17</v>
       </c>
@@ -1047,8 +1047,8 @@
       <c r="I7" s="25">
         <v>15</v>
       </c>
-      <c r="K7" s="29"/>
-      <c r="L7" s="34"/>
+      <c r="K7" s="28"/>
+      <c r="L7" s="33"/>
       <c r="R7" s="3"/>
     </row>
     <row r="8" spans="2:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1074,8 +1074,8 @@
       <c r="I8" s="25">
         <v>7</v>
       </c>
-      <c r="K8" s="29"/>
-      <c r="L8" s="34"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="33"/>
       <c r="R8" s="3" t="s">
         <v>19</v>
       </c>
@@ -1103,8 +1103,8 @@
       <c r="I9" s="25">
         <v>7</v>
       </c>
-      <c r="K9" s="29"/>
-      <c r="L9" s="34"/>
+      <c r="K9" s="28"/>
+      <c r="L9" s="33"/>
       <c r="R9" s="3" t="s">
         <v>20</v>
       </c>
@@ -1132,8 +1132,8 @@
       <c r="I10" s="25">
         <v>3</v>
       </c>
-      <c r="K10" s="29"/>
-      <c r="L10" s="34"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="33"/>
     </row>
     <row r="11" spans="2:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="10" t="str">
@@ -1158,8 +1158,8 @@
       <c r="I11" s="25">
         <v>5</v>
       </c>
-      <c r="K11" s="29"/>
-      <c r="L11" s="34"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="33"/>
     </row>
     <row r="12" spans="2:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="str">
@@ -1176,8 +1176,8 @@
       <c r="G12" s="19"/>
       <c r="H12" s="24"/>
       <c r="I12" s="25"/>
-      <c r="K12" s="29"/>
-      <c r="L12" s="34"/>
+      <c r="K12" s="28"/>
+      <c r="L12" s="33"/>
     </row>
     <row r="13" spans="2:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="10" t="str">
@@ -1194,8 +1194,8 @@
       <c r="G13" s="19"/>
       <c r="H13" s="24"/>
       <c r="I13" s="25"/>
-      <c r="K13" s="29"/>
-      <c r="L13" s="34"/>
+      <c r="K13" s="28"/>
+      <c r="L13" s="33"/>
     </row>
     <row r="14" spans="2:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10" t="str">
@@ -1212,8 +1212,8 @@
       <c r="G14" s="19"/>
       <c r="H14" s="24"/>
       <c r="I14" s="25"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="34"/>
+      <c r="K14" s="28"/>
+      <c r="L14" s="33"/>
     </row>
     <row r="15" spans="2:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="10" t="str">
@@ -1230,8 +1230,8 @@
       <c r="G15" s="19"/>
       <c r="H15" s="24"/>
       <c r="I15" s="25"/>
-      <c r="K15" s="29"/>
-      <c r="L15" s="34"/>
+      <c r="K15" s="28"/>
+      <c r="L15" s="33"/>
     </row>
     <row r="16" spans="2:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B16" s="10" t="str">
@@ -1248,8 +1248,8 @@
       <c r="G16" s="19"/>
       <c r="H16" s="24"/>
       <c r="I16" s="25"/>
-      <c r="K16" s="30"/>
-      <c r="L16" s="35"/>
+      <c r="K16" s="29"/>
+      <c r="L16" s="34"/>
     </row>
     <row r="17" spans="2:9" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10" t="str">

</xml_diff>

<commit_message>
[refactor] - time tracking
</commit_message>
<xml_diff>
--- a/src/main/resources/Boards Cutter template.xlsx
+++ b/src/main/resources/Boards Cutter template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Igor\Programming\Boards Cutter\BoardsCutter\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21E78497-147A-49A6-B873-07764E8254DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FEF01F-3AD4-46A7-AD8F-79FD33FC3189}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-75" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28455" yWindow="915" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Материалы</t>
   </si>
@@ -91,21 +91,6 @@
     <t>П-3</t>
   </si>
   <si>
-    <t>О-1</t>
-  </si>
-  <si>
-    <t>О-2</t>
-  </si>
-  <si>
-    <t>ОБ-1</t>
-  </si>
-  <si>
-    <t>ОБ-2</t>
-  </si>
-  <si>
-    <t>200х200</t>
-  </si>
-  <si>
     <t>Ячейки для заполнения - зеленые</t>
   </si>
   <si>
@@ -137,7 +122,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,6 +136,12 @@
       <name val="Bookman Old Style"/>
       <family val="1"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -876,8 +867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:E11"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -897,7 +888,7 @@
     <row r="1" spans="2:18" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:18" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B2" s="35" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C2" s="35"/>
       <c r="D2" s="35"/>
@@ -923,7 +914,7 @@
     </row>
     <row r="4" spans="2:18" ht="19.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>1</v>
@@ -932,7 +923,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="F4" s="5" t="s">
         <v>5</v>
@@ -947,10 +938,10 @@
         <v>7</v>
       </c>
       <c r="K4" s="31" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="L4" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="2:18" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
@@ -958,7 +949,7 @@
         <v>1</v>
       </c>
       <c r="C5" s="13" t="str" cm="1">
-        <f t="array" ref="C5:C7">_xlfn.UNIQUE(G5:G60,0,0)</f>
+        <f t="array" ref="C5:C6">_xlfn.UNIQUE(G5:G60,0,0)</f>
         <v>50х150</v>
       </c>
       <c r="D5" s="6">
@@ -980,26 +971,24 @@
         <v>15</v>
       </c>
       <c r="K5" s="30" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="L5" s="32">
         <v>0</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="2:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="10">
+      <c r="B6" s="10" t="str">
         <f>IF(AND(C6&lt;&gt;"",C6&lt;&gt;0),B5+1,"")</f>
-        <v>2</v>
-      </c>
-      <c r="C6" s="14" t="str">
-        <v>200х200</v>
-      </c>
-      <c r="D6" s="7">
-        <v>6000</v>
-      </c>
+        <v/>
+      </c>
+      <c r="C6" s="14">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7"/>
       <c r="E6" s="10">
         <f>IF(F6&lt;&gt;"",E5+1,"")</f>
         <v>2</v>
@@ -1019,7 +1008,7 @@
       <c r="K6" s="28"/>
       <c r="L6" s="33"/>
       <c r="R6" s="3" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1027,9 +1016,7 @@
         <f t="shared" ref="B7:B60" si="0">IF(AND(C7&lt;&gt;"",C7&lt;&gt;0),B6+1,"")</f>
         <v/>
       </c>
-      <c r="C7" s="14">
-        <v>0</v>
-      </c>
+      <c r="C7" s="14"/>
       <c r="D7" s="7"/>
       <c r="E7" s="10">
         <f t="shared" ref="E7:E60" si="1">IF(F7&lt;&gt;"",E6+1,"")</f>
@@ -1042,7 +1029,7 @@
         <v>3</v>
       </c>
       <c r="H7" s="24">
-        <v>1125</v>
+        <v>200</v>
       </c>
       <c r="I7" s="25">
         <v>15</v>
@@ -1058,26 +1045,18 @@
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="7"/>
-      <c r="E8" s="10">
-        <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="F8" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="H8" s="24">
-        <v>3000</v>
-      </c>
-      <c r="I8" s="25">
-        <v>7</v>
-      </c>
+      <c r="E8" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F8" s="18"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="25"/>
       <c r="K8" s="28"/>
       <c r="L8" s="33"/>
       <c r="R8" s="3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1087,26 +1066,18 @@
       </c>
       <c r="C9" s="14"/>
       <c r="D9" s="7"/>
-      <c r="E9" s="10">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="F9" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" s="19" t="s">
-        <v>3</v>
-      </c>
-      <c r="H9" s="24">
-        <v>4000</v>
-      </c>
-      <c r="I9" s="25">
-        <v>7</v>
-      </c>
+      <c r="E9" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F9" s="18"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="25"/>
       <c r="K9" s="28"/>
       <c r="L9" s="33"/>
       <c r="R9" s="3" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -1116,22 +1087,14 @@
       </c>
       <c r="C10" s="14"/>
       <c r="D10" s="7"/>
-      <c r="E10" s="10">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="F10" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="24">
-        <v>6000</v>
-      </c>
-      <c r="I10" s="25">
-        <v>3</v>
-      </c>
+      <c r="E10" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F10" s="18"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="25"/>
       <c r="K10" s="28"/>
       <c r="L10" s="33"/>
     </row>
@@ -1142,22 +1105,14 @@
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="7"/>
-      <c r="E11" s="10">
-        <f t="shared" si="1"/>
-        <v>7</v>
-      </c>
-      <c r="F11" s="18" t="s">
-        <v>14</v>
-      </c>
-      <c r="G11" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="H11" s="24">
-        <v>3500</v>
-      </c>
-      <c r="I11" s="25">
-        <v>5</v>
-      </c>
+      <c r="E11" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="F11" s="18"/>
+      <c r="G11" s="19"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="25"/>
       <c r="K11" s="28"/>
       <c r="L11" s="33"/>
     </row>
@@ -1962,6 +1917,7 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="E3:I3"/>
   </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="C5:C60">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>

</xml_diff>